<commit_message>
update allergies audio and separate prior illnesses
</commit_message>
<xml_diff>
--- a/medical-book/data.xlsx
+++ b/medical-book/data.xlsx
@@ -1,28 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cantonese-medical-handbook\medical-book\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248EECB-0A8B-46C4-8915-224A9E9D43F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="introductions" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="complaints" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="history_questions" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="prior_illnesses" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="family_history" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="medications" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="allergies" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="cardiology" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="dermatology" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="endocrinology" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="gastroenterology" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="general dentistry" sheetId="12" r:id="rId15"/>
+    <sheet name="introductions" sheetId="1" r:id="rId1"/>
+    <sheet name="complaints" sheetId="2" r:id="rId2"/>
+    <sheet name="history_questions" sheetId="3" r:id="rId3"/>
+    <sheet name="prior_illnesses" sheetId="4" r:id="rId4"/>
+    <sheet name="family_history" sheetId="5" r:id="rId5"/>
+    <sheet name="medications" sheetId="6" r:id="rId6"/>
+    <sheet name="allergies" sheetId="7" r:id="rId7"/>
+    <sheet name="cardiology" sheetId="8" r:id="rId8"/>
+    <sheet name="dermatology" sheetId="9" r:id="rId9"/>
+    <sheet name="endocrinology" sheetId="10" r:id="rId10"/>
+    <sheet name="gastroenterology" sheetId="11" r:id="rId11"/>
+    <sheet name="general dentistry" sheetId="12" r:id="rId12"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="452">
   <si>
     <t>Introduction and General Phrases</t>
   </si>
@@ -887,39 +909,6 @@
     <t>Allergies (Gwo3 man5)</t>
   </si>
   <si>
-    <t>Do you have any allergies to ?
-Medicines (antibodies) Food
-Other things</t>
-  </si>
-  <si>
-    <t>Nei5 deoi3 jau5 mou5 gwo3 man5?
-Joek6 mat6
-Sik6 mat6 
-Kei4 taa1 je5</t>
-  </si>
-  <si>
-    <t>你對___有冇過敏？
-藥物，食物，其他嘢？</t>
-  </si>
-  <si>
-    <t>Which medicines/ food?</t>
-  </si>
-  <si>
-    <t>Mat1 je5 joek6/ sik6 mat6?</t>
-  </si>
-  <si>
-    <t>乜嘢藥／食物？</t>
-  </si>
-  <si>
-    <t>What happens?</t>
-  </si>
-  <si>
-    <t>Jau5 mat1 je5 faan2 jing3?</t>
-  </si>
-  <si>
-    <t>有乜嘢反應？</t>
-  </si>
-  <si>
     <t>Rashes?</t>
   </si>
   <si>
@@ -945,24 +934,6 @@
   </si>
   <si>
     <t>你食過乜嘢抗生素？</t>
-  </si>
-  <si>
-    <t>Do you have any allergy medications?</t>
-  </si>
-  <si>
-    <t>Nei5 jau5 mou5 gwo3 man5 ge3 joek6 mat6 ？</t>
-  </si>
-  <si>
-    <t>你有冇過敏嘅藥物？</t>
-  </si>
-  <si>
-    <t>Have you had penicillin?</t>
-  </si>
-  <si>
-    <t>Nei5 jau5 mou5 sik6 gwo3 pun4 lei4 sai1 lam4?</t>
-  </si>
-  <si>
-    <t>你有無食過盤尼西林？</t>
   </si>
   <si>
     <t>Cardiology (Sam1 fo1)</t>
@@ -1488,15 +1459,45 @@
   </si>
   <si>
     <t>Kui2 joeng4</t>
+  </si>
+  <si>
+    <t>你對藥物，食物，同其他嘢有冇過敏？</t>
+  </si>
+  <si>
+    <t>penicillin / pun4 lei4 sai1 lam4 / 盤尼西林</t>
+  </si>
+  <si>
+    <t>What is your reaction?</t>
+  </si>
+  <si>
+    <t>Nei5 jau5 me1 faan2 jing3?</t>
+  </si>
+  <si>
+    <t>你有咩反應？</t>
+  </si>
+  <si>
+    <t>Are you taking any allergy medications?</t>
+  </si>
+  <si>
+    <t>Nei5 jau5 mou5 sik6 gan2 kong3 man5 ge3 joek6 mat6？</t>
+  </si>
+  <si>
+    <t>你有冇食緊抗敏嘅藥物？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have any allergies to medication, food, or other things? </t>
+  </si>
+  <si>
+    <t>Nei5 deoi3 joek6 mat6, sik6 mat6, tung4 kei4 taa1 je5 jau5 mou5  gwo3 man5?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -1504,105 +1505,125 @@
     <font>
       <b/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF212529"/>
       <name val="Roboto"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF6D9DEB"/>
       <name val="Georgia"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Cambria Math&quot;"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF6D9DEB"/>
       <name val="Georgia"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF6D9DEB"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF6D9DEB"/>
       <name val="Georgia"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF6D9DEB"/>
       <name val="Georgia"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1610,7 +1631,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1626,7 +1647,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -1640,163 +1667,122 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1986,25 +1972,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="13.8">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="27.6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2021,9 +2010,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="27.6">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -2035,9 +2024,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="27.6">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A25" si="1">A3+1</f>
+        <f t="shared" ref="A4:A25" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2050,9 +2039,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="41.4">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2065,9 +2054,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="27.6">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2080,9 +2069,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="82.8">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2095,9 +2084,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="13.8">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2110,9 +2099,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="27.6">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2125,9 +2114,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="41.4">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2140,9 +2129,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="41.4">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2155,9 +2144,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="41.4">
       <c r="A12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2170,9 +2159,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="13.8">
       <c r="A13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2185,9 +2174,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="41.4">
       <c r="A14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -2200,9 +2189,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="27.6">
       <c r="A15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -2215,9 +2204,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="27.6">
       <c r="A16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -2230,9 +2219,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="55.2">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -2245,9 +2234,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="41.4">
       <c r="A18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -2260,9 +2249,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="41.4">
       <c r="A19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -2275,9 +2264,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="15.6">
       <c r="A20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2290,9 +2279,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" ht="67.5" customHeight="1">
+    <row r="21" spans="1:4" ht="67.5" customHeight="1">
       <c r="A21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -2305,9 +2294,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.6">
       <c r="A22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2320,9 +2309,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="15.6">
       <c r="A23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2335,9 +2324,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.6">
       <c r="A24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2350,9 +2339,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="15.6">
       <c r="A25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2366,37 +2355,38 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="21"/>
-    </row>
-    <row r="3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2404,47 +2394,47 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="28" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="22"/>
-    </row>
-    <row r="12">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -2452,121 +2442,122 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="6" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="22"/>
-    </row>
-    <row r="20">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="21"/>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="22"/>
-    </row>
-    <row r="22">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>395</v>
+        <v>379</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="21"/>
-    </row>
-    <row r="3">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2574,93 +2565,93 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="22"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="24"/>
-    </row>
-    <row r="17">
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="23"/>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="22"/>
-    </row>
-    <row r="19">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2668,42 +2659,42 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="6" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="22"/>
-    </row>
-    <row r="24">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="21"/>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="22"/>
-    </row>
-    <row r="26">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2711,98 +2702,98 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="B27" s="6" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="B28" s="6" t="s">
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="22"/>
-    </row>
-    <row r="38">
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="22"/>
-    </row>
-    <row r="40">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -2810,123 +2801,125 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2">
       <c r="A41" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="23"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="23"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="B41" s="6" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="6" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="22"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="24"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="24"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="6" t="s">
-        <v>449</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>456</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2943,9 +2936,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>75</v>
@@ -2957,9 +2950,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A15" si="1">A3+1</f>
+        <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2972,9 +2965,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2987,9 +2980,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3002,9 +2995,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3017,9 +3010,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3032,9 +3025,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3047,9 +3040,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3062,9 +3055,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -3077,9 +3070,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -3092,9 +3085,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -3107,9 +3100,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3122,9 +3115,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -3138,26 +3131,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="C1" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3171,9 +3165,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>115</v>
@@ -3185,9 +3179,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A17" si="1">A3+1</f>
+        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -3200,9 +3194,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3215,9 +3209,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3230,9 +3224,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3245,9 +3239,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3260,9 +3254,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3275,9 +3269,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -3290,9 +3284,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -3305,9 +3299,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4">
       <c r="A12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -3320,9 +3314,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4">
       <c r="A13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -3335,9 +3329,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4">
       <c r="A14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -3350,9 +3344,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4">
       <c r="A15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -3365,9 +3359,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4">
       <c r="A16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -3380,9 +3374,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -3396,26 +3390,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="C1" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3429,9 +3424,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>160</v>
@@ -3443,9 +3438,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A18" si="1">A3+1</f>
+        <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -3458,9 +3453,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3473,9 +3468,9 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3488,9 +3483,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3503,9 +3498,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3518,9 +3513,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3533,9 +3528,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3548,9 +3543,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -3563,9 +3558,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4">
       <c r="A12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -3578,9 +3573,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4">
       <c r="A13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -3593,9 +3588,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4">
       <c r="A14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3608,9 +3603,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4">
       <c r="A15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -3623,9 +3618,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4">
       <c r="A16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -3638,9 +3633,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3653,9 +3648,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4">
       <c r="A18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -3669,26 +3664,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="C1" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3702,9 +3698,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>209</v>
@@ -3716,9 +3712,9 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
+        <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -3731,9 +3727,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3746,9 +3742,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3761,9 +3757,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3776,9 +3772,9 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3791,9 +3787,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3806,9 +3802,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -3822,27 +3818,30 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="29" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -3859,9 +3858,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>234</v>
@@ -3873,9 +3872,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A11" si="1">A3+1</f>
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -3888,9 +3887,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3903,9 +3902,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3918,9 +3917,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3933,9 +3932,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3948,9 +3947,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -3963,9 +3962,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3978,9 +3977,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -3997,26 +3996,29 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="C1" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="41.4">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -4030,515 +4032,500 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5">
-        <v>1.0</v>
+    <row r="3" spans="1:5" ht="96.6">
+      <c r="A3" s="31">
+        <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="41.4">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27.6">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="6" spans="1:5" ht="55.2">
+      <c r="A6" s="31">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="15" t="s">
+    <row r="7" spans="1:5" ht="55.2">
+      <c r="A7" s="31">
+        <f t="shared" ref="A5:A8" si="0">A6+1</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C7" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D7" s="15" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5">
-        <f t="shared" si="1"/>
+    <row r="8" spans="1:5" ht="69">
+      <c r="A8" s="31">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>278</v>
+        <v>447</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>448</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>285</v>
-      </c>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="21"/>
-    </row>
-    <row r="3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6">
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="22"/>
-    </row>
-    <row r="10">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="22"/>
-    </row>
-    <row r="12">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="23"/>
-    </row>
-    <row r="13">
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="23"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="23"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="22"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="24"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="24"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C22" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="10" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C23" s="6" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="10" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="23"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="24"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="17" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="22"/>
-    </row>
-    <row r="27">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="21"/>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="23"/>
-    </row>
-    <row r="28">
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="6" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="C28" s="26"/>
-    </row>
-    <row r="29">
+        <v>309</v>
+      </c>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="22"/>
-    </row>
-    <row r="31">
+        <v>311</v>
+      </c>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="22"/>
-    </row>
-    <row r="33">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="23"/>
-    </row>
-    <row r="34">
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C34" s="26"/>
-    </row>
-    <row r="35">
+        <v>314</v>
+      </c>
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36">
+        <v>316</v>
+      </c>
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="C36" s="26"/>
-    </row>
-    <row r="37">
+        <v>318</v>
+      </c>
+      <c r="C36" s="25"/>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="C37" s="26"/>
-    </row>
-    <row r="38">
+        <v>320</v>
+      </c>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C38" s="26"/>
-    </row>
-    <row r="39">
+        <v>322</v>
+      </c>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C39" s="26"/>
+        <v>324</v>
+      </c>
+      <c r="C39" s="25"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="21"/>
-    </row>
-    <row r="3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6">
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C6" s="26"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="22"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="24"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="24"/>
-    </row>
-    <row r="10">
+        <v>327</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="23"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="10" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="C10" s="27"/>
-    </row>
-    <row r="11">
+        <v>329</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="C11" s="27"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="24"/>
-    </row>
-    <row r="13">
+        <v>331</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="23"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="22"/>
-    </row>
-    <row r="15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -4546,90 +4533,90 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B16" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="22"/>
-    </row>
-    <row r="26">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="22"/>
-    </row>
-    <row r="28">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -4637,31 +4624,31 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="6" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added cardiology page, hidden from navbar for now
</commit_message>
<xml_diff>
--- a/medical-book/data.xlsx
+++ b/medical-book/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cantonese-medical-handbook\medical-book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248EECB-0A8B-46C4-8915-224A9E9D43F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB96A5C0-93C0-45A3-817E-673BCDB31F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="introductions" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,13 @@
     <sheet name="family_history" sheetId="5" r:id="rId5"/>
     <sheet name="medications" sheetId="6" r:id="rId6"/>
     <sheet name="allergies" sheetId="7" r:id="rId7"/>
-    <sheet name="cardiology" sheetId="8" r:id="rId8"/>
-    <sheet name="dermatology" sheetId="9" r:id="rId9"/>
-    <sheet name="endocrinology" sheetId="10" r:id="rId10"/>
-    <sheet name="gastroenterology" sheetId="11" r:id="rId11"/>
-    <sheet name="general dentistry" sheetId="12" r:id="rId12"/>
+    <sheet name="cardiology" sheetId="13" r:id="rId8"/>
+    <sheet name="cardiovascular_illnesses" sheetId="14" r:id="rId9"/>
+    <sheet name="cardiology_orig" sheetId="8" r:id="rId10"/>
+    <sheet name="dermatology" sheetId="9" r:id="rId11"/>
+    <sheet name="endocrinology" sheetId="10" r:id="rId12"/>
+    <sheet name="gastroenterology" sheetId="11" r:id="rId13"/>
+    <sheet name="general dentistry" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="464">
   <si>
     <t>Introduction and General Phrases</t>
   </si>
@@ -1489,6 +1491,42 @@
   </si>
   <si>
     <t>Nei5 deoi3 joek6 mat6, sik6 mat6, tung4 kei4 taa1 je5 jau5 mou5  gwo3 man5?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam1 gwai3 </t>
+  </si>
+  <si>
+    <t>心悸</t>
+  </si>
+  <si>
+    <t>心跳呒规律</t>
+  </si>
+  <si>
+    <t>cardiovascular illnesses</t>
+  </si>
+  <si>
+    <t>see more</t>
+  </si>
+  <si>
+    <t>冠心病</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam1 zong6 beng6 </t>
+  </si>
+  <si>
+    <t>心脏病</t>
+  </si>
+  <si>
+    <t>心力衰竭</t>
+  </si>
+  <si>
+    <t>高胆固醇血症</t>
+  </si>
+  <si>
+    <t>高血压</t>
+  </si>
+  <si>
+    <t>心肌梗塞</t>
   </si>
 </sst>
 </file>
@@ -1753,10 +1791,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1764,6 +1798,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2360,6 +2398,520 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="23"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="23"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="21"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C36" s="25"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C39" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="23"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="23"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2530,7 +3082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2887,7 +3439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3835,11 +4387,11 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="18" t="s">
@@ -4007,13 +4559,13 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="13.8">
       <c r="C1" s="1" t="s">
         <v>261</v>
       </c>
@@ -4033,7 +4585,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="96.6">
-      <c r="A3" s="31">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -4045,12 +4597,12 @@
       <c r="D3" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="30" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="41.4">
-      <c r="A4" s="31">
+      <c r="A4" s="29">
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -4064,7 +4616,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="27.6">
-      <c r="A5" s="31">
+      <c r="A5" s="29">
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -4078,7 +4630,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="55.2">
-      <c r="A6" s="31">
+      <c r="A6" s="29">
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -4092,8 +4644,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="55.2">
-      <c r="A7" s="31">
-        <f t="shared" ref="A5:A8" si="0">A6+1</f>
+      <c r="A7" s="29">
+        <f t="shared" ref="A7:A8" si="0">A6+1</f>
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -4107,14 +4659,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="69">
-      <c r="A8" s="31">
+      <c r="A8" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>447</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>448</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -4140,302 +4692,218 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:C39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9579C6-1115-44BF-8A2B-115FE4524D3E}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="18"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="21"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C3" t="s">
         <v>274</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C4" t="s">
         <v>277</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C5" t="s">
         <v>280</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="21"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="21"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>283</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C8" t="s">
         <v>284</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D8" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="21"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="23"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="6" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C9" t="s">
         <v>287</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="D9" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>289</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C10" t="s">
         <v>290</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="10" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>292</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C11" t="s">
         <v>293</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D11" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="6" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>295</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C12" t="s">
         <v>296</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D12" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="10" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>298</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C13" t="s">
         <v>299</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D13" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="10" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>301</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C14" t="s">
         <v>302</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D14" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="6" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>304</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C15" t="s">
         <v>305</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D15" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="23"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="17" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="21"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="22"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="C28" s="25"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C29" s="25"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="21"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="17" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="21"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="22"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C34" s="25"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C35" s="25"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="C36" s="25"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="C37" s="25"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C38" s="25"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="C39" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4443,209 +4911,119 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BF51B-02B0-4E17-B944-DD7DD6C58694}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="18"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="21"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C6" s="25"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="21"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="23"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="21"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="21"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="17" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="21"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>355</v>
+      <c r="B4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" t="s">
+        <v>458</v>
+      </c>
+      <c r="D4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update audio, 8-23 meeting
</commit_message>
<xml_diff>
--- a/medical-book/data.xlsx
+++ b/medical-book/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cantonese-medical-handbook\medical-book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB96A5C0-93C0-45A3-817E-673BCDB31F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7697BB0D-F930-4B12-8441-188F68ACCD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="introductions" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="467">
   <si>
     <t>Introduction and General Phrases</t>
   </si>
@@ -773,12 +773,6 @@
     <t>What was the cause of death?</t>
   </si>
   <si>
-    <t>Keoi5 heoi3 sai3 ge3 si4 hau6 gei2 seoi3?</t>
-  </si>
-  <si>
-    <t>佢去世嘅時候幾歲？</t>
-  </si>
-  <si>
     <t>Do you have any siblings?</t>
   </si>
   <si>
@@ -896,16 +890,10 @@
     <t>Zung1 joek6 caa4</t>
   </si>
   <si>
-    <t>中藥茶</t>
-  </si>
-  <si>
     <t>Supplements/ Vitamins</t>
   </si>
   <si>
     <t>Bou2 gin3 ban2/Wai4 taa1 min6</t>
-  </si>
-  <si>
-    <t>保健品／維他命</t>
   </si>
   <si>
     <t>Allergies (Gwo3 man5)</t>
@@ -1527,6 +1515,31 @@
   </si>
   <si>
     <t>心肌梗塞</t>
+  </si>
+  <si>
+    <t>草本茶</t>
+  </si>
+  <si>
+    <t>保健品
+維他命</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was their age at their time of death? 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keoi5 heoi3 sai3 ge3 si4 hau6 gei2 seoi3? 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佢去世嘅時候幾歲？
+</t>
+  </si>
+  <si>
+    <t>Keoi5 ge3 sei4 jan1 hai6 me1?</t>
+  </si>
+  <si>
+    <t>佢嘅死因係咩?</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1802,6 +1815,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2410,7 +2435,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2418,7 +2443,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2435,35 +2460,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2471,7 +2496,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="17" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2488,13 +2513,13 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2508,79 +2533,79 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2588,7 +2613,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2605,19 +2630,19 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C29" s="25"/>
     </row>
@@ -2626,7 +2651,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2643,55 +2668,55 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C35" s="25"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C36" s="25"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C37" s="25"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C38" s="25"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C39" s="25"/>
     </row>
@@ -2713,7 +2738,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2721,7 +2746,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2738,10 +2763,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C6" s="25"/>
     </row>
@@ -2756,19 +2781,19 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C11" s="12"/>
     </row>
@@ -2777,7 +2802,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="17" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2793,74 +2818,74 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2868,7 +2893,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2884,26 +2909,26 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2924,7 +2949,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2932,7 +2957,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2948,39 +2973,39 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="26" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2996,50 +3021,50 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3047,7 +3072,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3063,18 +3088,18 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3120,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3103,7 +3128,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3119,74 +3144,74 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="6" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="6" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3197,7 +3222,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="17" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3213,26 +3238,26 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3240,7 +3265,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3256,82 +3281,82 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="6" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="6" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3339,7 +3364,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3355,42 +3380,42 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="6" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="6" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3404,34 +3429,34 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="6" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="6" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -4225,9 +4250,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -4251,122 +4278,137 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="34" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <f t="shared" ref="A4:A10" si="0">A3+1</f>
+      <c r="A4" s="29">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="34" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5">
+      <c r="A5" s="29">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="29">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C6" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="C7" s="34" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="D7" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="6" t="s">
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="29">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C8" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="D8" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="C9" s="34" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="D9" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C10" s="34" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="D10" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C9" s="6" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" s="29">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="C11" s="35" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="D11" s="35" t="s">
         <v>230</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4381,14 +4423,16 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
@@ -4415,13 +4459,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4430,13 +4474,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4445,13 +4489,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4460,13 +4504,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4475,13 +4519,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>246</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4490,13 +4534,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>249</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4505,43 +4549,43 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C9" s="15" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="27.6">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="15" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="41.4">
+      <c r="A11" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C11" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>259</v>
-      </c>
       <c r="D11" s="15" t="s">
-        <v>260</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4567,7 +4611,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.8">
       <c r="C1" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="41.4">
@@ -4589,16 +4633,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="41.4">
@@ -4606,13 +4650,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27.6">
@@ -4620,13 +4664,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="55.2">
@@ -4634,13 +4678,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="55.2">
@@ -4649,13 +4693,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="69">
@@ -4664,13 +4708,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8">
@@ -4703,7 +4747,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4720,7 +4764,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4728,13 +4772,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4742,13 +4786,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4756,13 +4800,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4770,13 +4814,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D6" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4784,13 +4828,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D7" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4798,13 +4842,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4812,13 +4856,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C9" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4826,13 +4870,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4840,13 +4884,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4854,13 +4898,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4868,13 +4912,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C13" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4882,13 +4926,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C14" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D14" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4896,13 +4940,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4914,7 +4958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BF51B-02B0-4E17-B944-DD7DD6C58694}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4922,7 +4966,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4939,7 +4983,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4947,13 +4991,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4961,13 +5005,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C4" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D4" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4975,13 +5019,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4989,13 +5033,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5003,13 +5047,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D7" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5017,13 +5061,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D8" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>